<commit_message>
Update app.py with Top 5 tables
</commit_message>
<xml_diff>
--- a/Stierenkaart/April/Basislijst stierenoverzicvht.xlsx
+++ b/Stierenkaart/April/Basislijst stierenoverzicvht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kisamen-my.sharepoint.com/personal/v_vanrooijen_kisamen_com/Documents/Bureaublad/Project Stierenkaart/Stierenkaart/April/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96742668-2720-495F-A1CF-B9ACCFC07F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{07DCA8EE-E184-47C3-945B-3AF214BA2219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32940" yWindow="2244" windowWidth="20748" windowHeight="13392" xr2:uid="{EA99E83E-538F-4F06-AEBD-9593C8BA2E23}"/>
+    <workbookView xWindow="-30840" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{EA99E83E-538F-4F06-AEBD-9593C8BA2E23}"/>
   </bookViews>
   <sheets>
     <sheet name="Fokstieren stierenkaart" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>KI-code</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Stier ZWARTBONT</t>
+  </si>
+  <si>
+    <t>AMERICAN FLORIAN</t>
   </si>
 </sst>
 </file>
@@ -612,19 +615,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A22A848-A962-468F-AB98-A9A4D762EBF3}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>782666</v>
       </c>
@@ -640,7 +643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>361096</v>
       </c>
@@ -648,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>361218</v>
       </c>
@@ -656,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>780644</v>
       </c>
@@ -664,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>361189</v>
       </c>
@@ -672,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>361221</v>
       </c>
@@ -680,7 +683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>361219</v>
       </c>
@@ -688,7 +691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>361197</v>
       </c>
@@ -699,7 +702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>361191</v>
       </c>
@@ -710,7 +713,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>781289</v>
       </c>
@@ -718,7 +721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>361170</v>
       </c>
@@ -726,7 +729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>361174</v>
       </c>
@@ -734,7 +737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>361112</v>
       </c>
@@ -742,7 +745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>361181</v>
       </c>
@@ -753,7 +756,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>361184</v>
       </c>
@@ -761,158 +764,166 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>361226</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>361186</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>781489</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>361190</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>782891</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>783404</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>782492</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>361198</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>361134</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>361052</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>361216</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>361151</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>780396</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>361214</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>361092</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>361171</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>361222</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>361145</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>361242</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>361231</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>35</v>
       </c>
     </row>
@@ -926,12 +937,12 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,7 +950,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>365008</v>
       </c>
@@ -947,7 +958,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>784268</v>
       </c>
@@ -955,7 +966,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>783761</v>
       </c>
@@ -963,7 +974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>785140</v>
       </c>
@@ -971,7 +982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>784494</v>
       </c>
@@ -979,7 +990,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>784695</v>
       </c>
@@ -987,7 +998,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>784058</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>783460</v>
       </c>
@@ -1003,7 +1014,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>785456</v>
       </c>
@@ -1011,7 +1022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>783482</v>
       </c>
@@ -1019,7 +1030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>783760</v>
       </c>
@@ -1027,7 +1038,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>784647</v>
       </c>
@@ -1035,7 +1046,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>785455</v>
       </c>
@@ -1043,7 +1054,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>783481</v>
       </c>
@@ -1051,7 +1062,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>783483</v>
       </c>
@@ -1059,7 +1070,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>784852</v>
       </c>
@@ -1067,7 +1078,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>361278</v>
       </c>
@@ -1075,7 +1086,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>361295</v>
       </c>
@@ -1083,7 +1094,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>361325</v>
       </c>
@@ -1091,7 +1102,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1110,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>783749</v>
       </c>
@@ -1107,7 +1118,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>784972</v>
       </c>
@@ -1115,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>784190</v>
       </c>
@@ -1123,7 +1134,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>785031</v>
       </c>
@@ -1131,7 +1142,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>784971</v>
       </c>
@@ -1139,7 +1150,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>786007</v>
       </c>
@@ -1147,7 +1158,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>784361</v>
       </c>
@@ -1155,7 +1166,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>783461</v>
       </c>
@@ -1163,7 +1174,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>785040</v>
       </c>
@@ -1171,7 +1182,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>361285</v>
       </c>

</xml_diff>